<commit_message>
test: Validar Ativos únicos
</commit_message>
<xml_diff>
--- a/extract/data/excel_source/Asset.xlsx
+++ b/extract/data/excel_source/Asset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\facilitador_de_aporte_mensal\extract\data\excel_source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF20261-AB07-4810-A998-E0CB27F7022D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F72ABD-05BB-4AE1-9158-FC3A10591A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3D31D9D7-E687-4EE0-8E8B-1A62F06EF521}"/>
   </bookViews>
@@ -51,40 +51,40 @@
     <t>SUZB3</t>
   </si>
   <si>
+    <t>BBSA3</t>
+  </si>
+  <si>
+    <t>TRPL4</t>
+  </si>
+  <si>
+    <t>KNCR11</t>
+  </si>
+  <si>
+    <t>BBSE3</t>
+  </si>
+  <si>
+    <t>HGLG11</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>CARTEIRA</t>
+  </si>
+  <si>
+    <t>TAEE4</t>
+  </si>
+  <si>
+    <t>MONITORAMENTO</t>
+  </si>
+  <si>
+    <t>CXSE3</t>
+  </si>
+  <si>
+    <t>ASSET</t>
+  </si>
+  <si>
     <t>CPLE6</t>
-  </si>
-  <si>
-    <t>BBSA3</t>
-  </si>
-  <si>
-    <t>TRPL4</t>
-  </si>
-  <si>
-    <t>KNCR11</t>
-  </si>
-  <si>
-    <t>BBSE3</t>
-  </si>
-  <si>
-    <t>HGLG11</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>CARTEIRA</t>
-  </si>
-  <si>
-    <t>TAEE4</t>
-  </si>
-  <si>
-    <t>MONITORAMENTO</t>
-  </si>
-  <si>
-    <t>CXSE3</t>
-  </si>
-  <si>
-    <t>ASSET</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F11D4F-2DA7-4755-B563-3E265DD32F4E}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -447,10 +449,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -458,7 +460,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -466,7 +468,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -474,7 +476,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -482,7 +484,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -490,71 +492,71 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>